<commit_message>
permutation logic is added in matrix calculation
</commit_message>
<xml_diff>
--- a/3. MicroService/reports/observ/matrix.xlsx
+++ b/3. MicroService/reports/observ/matrix.xlsx
@@ -749,14 +749,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>-1</t>
@@ -769,7 +769,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -857,19 +857,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>-1</t>
@@ -877,12 +877,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -897,12 +897,12 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -917,12 +917,12 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -937,12 +937,12 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -965,37 +965,37 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1005,17 +1005,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -1025,17 +1025,17 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1045,17 +1045,17 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1185,34 +1185,34 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="I9" t="inlineStr">
         <is>
           <t>-1</t>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -1293,39 +1293,39 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>-1</t>
@@ -1333,12 +1333,12 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1353,12 +1353,12 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1373,12 +1373,12 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1401,57 +1401,57 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1461,17 +1461,17 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1481,17 +1481,17 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1621,54 +1621,54 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="M13" t="inlineStr">
         <is>
           <t>-1</t>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -1729,59 +1729,59 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="N14" t="inlineStr">
         <is>
           <t>-1</t>
@@ -1789,12 +1789,12 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -1809,12 +1809,12 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
@@ -1837,77 +1837,77 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1917,17 +1917,17 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -2057,74 +2057,74 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="Q17" t="inlineStr">
         <is>
           <t>-1</t>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
@@ -2165,79 +2165,79 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="R18" t="inlineStr">
         <is>
           <t>-1</t>
@@ -2245,12 +2245,12 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
@@ -2273,97 +2273,97 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2493,12 +2493,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2513,12 +2513,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2533,12 +2533,12 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -2553,12 +2553,12 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -2601,17 +2601,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2621,17 +2621,17 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2641,17 +2641,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -2661,17 +2661,17 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2681,12 +2681,12 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
@@ -2709,97 +2709,97 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>N</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">

</xml_diff>